<commit_message>
VMC and Prime Video Test Cases
</commit_message>
<xml_diff>
--- a/FlipApp/testdata/userdata.xlsx
+++ b/FlipApp/testdata/userdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhupesh\git\flip-app\FlipApp\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarungoswami/git/flip-app/FlipApp/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CFC10F-C01B-42D4-85B1-85577972E541}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E38CD5-509C-2646-8F7E-1ECBD641B58A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="49">
   <si>
     <t>Role</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>vinay2.guest</t>
+  </si>
+  <si>
+    <t>Guru</t>
+  </si>
+  <si>
+    <t>parul.s</t>
   </si>
 </sst>
 </file>
@@ -518,20 +524,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="10.69921875"/>
+    <col min="1" max="6" width="10.6640625"/>
     <col min="7" max="7" width="20"/>
-    <col min="8" max="1025" width="10.69921875"/>
+    <col min="8" max="1025" width="10.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +563,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -583,7 +589,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -609,7 +615,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -635,7 +641,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -661,7 +667,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -687,7 +693,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -713,7 +719,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -739,7 +745,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -765,7 +771,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -791,7 +797,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -817,7 +823,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -843,7 +849,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -869,7 +875,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -895,7 +901,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -921,7 +927,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -947,7 +953,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -973,7 +979,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -999,7 +1005,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1025,7 +1031,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1051,7 +1057,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1077,7 +1083,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1103,7 +1109,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1129,7 +1135,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1155,7 +1161,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1181,7 +1187,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1207,7 +1213,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -1233,7 +1239,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1285,7 +1291,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1311,7 +1317,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -1337,7 +1343,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -1360,6 +1366,32 @@
         <v>46</v>
       </c>
       <c r="H32" s="1">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="1">
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H33" s="1">
         <v>123456</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed TC for DisplayVMCStudent
</commit_message>
<xml_diff>
--- a/FlipApp/testdata/userdata.xlsx
+++ b/FlipApp/testdata/userdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarungoswami/git/flip-app/FlipApp/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhupesh\git\flip-app\FlipApp\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E38CD5-509C-2646-8F7E-1ECBD641B58A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7C3A8F-8B8A-47B1-BA08-4549E0E5BD8F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -526,18 +526,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="10.6640625"/>
+    <col min="1" max="6" width="10.69921875"/>
     <col min="7" max="7" width="20"/>
-    <col min="8" max="1025" width="10.6640625"/>
+    <col min="8" max="1025" width="10.69921875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -563,7 +563,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -589,7 +589,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -615,7 +615,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -641,7 +641,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -667,7 +667,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -693,7 +693,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -719,7 +719,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -745,7 +745,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -771,7 +771,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -797,7 +797,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -823,7 +823,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -849,7 +849,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -875,7 +875,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -901,7 +901,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -927,7 +927,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -953,7 +953,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -979,7 +979,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F24" t="s">
         <v>13</v>
@@ -1161,7 +1161,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>21</v>
       </c>

</xml_diff>